<commit_message>
Merged in feature/ZG-188-服务端体力系统制作 (pull request #17)
Feature/ZG-188 服务端体力系统制作
</commit_message>
<xml_diff>
--- a/config/excel/CrystalLevelup.xlsx
+++ b/config/excel/CrystalLevelup.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12540"/>
+    <workbookView windowWidth="24225" windowHeight="12540"/>
   </bookViews>
   <sheets>
     <sheet name="CrystalLevelup" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>行列头两行不会被读取</t>
   </si>
@@ -32,9 +32,6 @@
   </si>
   <si>
     <t>exp</t>
-  </si>
-  <si>
-    <t>gold</t>
   </si>
   <si>
     <t>accountLevelLimit</t>
@@ -61,24 +58,6 @@
     <t>所需经验值</t>
   </si>
   <si>
-    <t>白品所需金币</t>
-  </si>
-  <si>
-    <t>绿品所需金币</t>
-  </si>
-  <si>
-    <t>蓝品所需金币</t>
-  </si>
-  <si>
-    <t>紫品所需金币</t>
-  </si>
-  <si>
-    <t>橙品所需金币</t>
-  </si>
-  <si>
-    <t>消耗金币</t>
-  </si>
-  <si>
     <t>账号等级限制</t>
   </si>
   <si>
@@ -99,8 +78,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
@@ -131,19 +110,31 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="0"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Helvetica Neue"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -155,31 +146,40 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -201,37 +201,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Helvetica Neue"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -245,19 +224,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -268,8 +239,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -308,55 +287,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -368,127 +455,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -546,39 +525,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -590,6 +536,17 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -620,10 +577,8 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -643,16 +598,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -661,133 +640,133 @@
     <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2011,10 +1990,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:P48"/>
+  <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7:O22"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="13.35" customHeight="1"/>
@@ -2024,13 +2003,12 @@
     <col min="3" max="3" width="8.5" style="1" customWidth="1"/>
     <col min="4" max="8" width="18.5416666666667" style="1" customWidth="1"/>
     <col min="9" max="9" width="36.4583333333333" style="1" customWidth="1"/>
-    <col min="10" max="14" width="12.5416666666667" style="1" customWidth="1"/>
-    <col min="15" max="15" width="36.4583333333333" style="1" customWidth="1"/>
-    <col min="16" max="16" width="17.7666666666667" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="6" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17.7666666666667" style="1" customWidth="1"/>
+    <col min="11" max="16378" width="6" style="1" customWidth="1"/>
+    <col min="16379" max="16384" width="6" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14" customHeight="1" spans="1:14">
+    <row r="1" ht="14" customHeight="1" spans="1:9">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2042,13 +2020,8 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-    </row>
-    <row r="2" ht="47" customHeight="1" spans="1:15">
+    </row>
+    <row r="2" ht="47" customHeight="1" spans="1:9">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="2" t="s">
@@ -2062,16 +2035,8 @@
       <c r="I2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" ht="16.15" customHeight="1" spans="1:16">
+    </row>
+    <row r="3" ht="16.15" customHeight="1" spans="1:10">
       <c r="A3" s="3"/>
       <c r="B3" s="2" t="s">
         <v>3</v>
@@ -2087,70 +2052,44 @@
       <c r="I3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4" t="s">
+      <c r="J3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" ht="16.15" customHeight="1" spans="1:16">
+    </row>
+    <row r="4" ht="16.15" customHeight="1" spans="1:10">
       <c r="A4" s="3"/>
       <c r="B4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="J4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" ht="16.15" customHeight="1" spans="1:16">
+    </row>
+    <row r="5" ht="16.15" customHeight="1" spans="1:10">
       <c r="A5" s="3"/>
       <c r="B5" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -2159,21 +2098,15 @@
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
-    </row>
-    <row r="6" ht="16.15" customHeight="1" spans="1:16">
+      <c r="J5" s="10"/>
+    </row>
+    <row r="6" ht="16.15" customHeight="1" spans="1:10">
       <c r="A6" s="3"/>
       <c r="B6" s="2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -2181,837 +2114,445 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="P6" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" ht="14.25" spans="1:16">
+        <v>18</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" ht="14.25" spans="1:10">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="5">
         <v>0</v>
       </c>
       <c r="D7" s="1">
-        <v>76</v>
+        <v>1201</v>
       </c>
       <c r="E7" s="1">
-        <v>101</v>
+        <v>1801</v>
       </c>
       <c r="F7" s="6">
-        <v>127</v>
+        <v>2401</v>
       </c>
       <c r="G7" s="1">
-        <v>152</v>
+        <v>3002</v>
       </c>
       <c r="H7" s="1">
-        <v>177</v>
+        <v>3602</v>
       </c>
       <c r="I7" s="1" t="str">
         <f>D7&amp;","&amp;E7&amp;","&amp;F7&amp;","&amp;G7&amp;","&amp;H7</f>
-        <v>76,101,127,152,177</v>
-      </c>
-      <c r="J7" s="1">
-        <f>D7*10</f>
-        <v>760</v>
-      </c>
-      <c r="K7" s="1">
-        <f t="shared" ref="K7:K22" si="0">E7*10</f>
-        <v>1010</v>
-      </c>
-      <c r="L7" s="1">
-        <f t="shared" ref="L7:L22" si="1">F7*10</f>
-        <v>1270</v>
-      </c>
-      <c r="M7" s="1">
-        <f t="shared" ref="M7:M22" si="2">G7*10</f>
-        <v>1520</v>
-      </c>
-      <c r="N7" s="1">
-        <f t="shared" ref="N7:N22" si="3">H7*10</f>
-        <v>1770</v>
-      </c>
-      <c r="O7" s="1" t="str">
-        <f>J7&amp;","&amp;K7&amp;","&amp;L7&amp;","&amp;M7&amp;","&amp;N7</f>
-        <v>760,1010,1270,1520,1770</v>
-      </c>
-      <c r="P7" s="6">
+        <v>1201,1801,2401,3002,3602</v>
+      </c>
+      <c r="J7" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="8" ht="14.25" spans="1:16">
+    <row r="8" ht="14.25" spans="1:10">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="5">
         <v>1</v>
       </c>
       <c r="D8" s="1">
-        <v>199</v>
+        <v>1034</v>
       </c>
       <c r="E8" s="1">
-        <v>265</v>
+        <v>1651</v>
       </c>
       <c r="F8" s="7">
-        <v>332</v>
+        <v>2268</v>
       </c>
       <c r="G8" s="1">
-        <v>398</v>
+        <v>2885</v>
       </c>
       <c r="H8" s="1">
-        <v>464</v>
+        <v>3502</v>
       </c>
       <c r="I8" s="1" t="str">
         <f>D8&amp;","&amp;E8&amp;","&amp;F8&amp;","&amp;G8&amp;","&amp;H8</f>
-        <v>199,265,332,398,464</v>
-      </c>
-      <c r="J8" s="1">
-        <f t="shared" ref="J8:J22" si="4">D8*10</f>
-        <v>1990</v>
-      </c>
-      <c r="K8" s="1">
-        <f t="shared" si="0"/>
-        <v>2650</v>
-      </c>
-      <c r="L8" s="1">
-        <f t="shared" si="1"/>
-        <v>3320</v>
-      </c>
-      <c r="M8" s="1">
-        <f t="shared" si="2"/>
-        <v>3980</v>
-      </c>
-      <c r="N8" s="1">
-        <f t="shared" si="3"/>
-        <v>4640</v>
-      </c>
-      <c r="O8" s="1" t="str">
-        <f>J8&amp;","&amp;K8&amp;","&amp;L8&amp;","&amp;M8&amp;","&amp;N8</f>
-        <v>1990,2650,3320,3980,4640</v>
-      </c>
-      <c r="P8" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" customHeight="1" spans="3:16">
+        <v>1034,1651,2268,2885,3502</v>
+      </c>
+      <c r="J8" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" customHeight="1" spans="3:10">
       <c r="C9" s="5">
         <v>2</v>
       </c>
       <c r="D9" s="1">
-        <v>658</v>
+        <v>2606</v>
       </c>
       <c r="E9" s="1">
-        <v>877</v>
+        <v>3909</v>
       </c>
       <c r="F9" s="7">
-        <v>1097</v>
+        <v>5212</v>
       </c>
       <c r="G9" s="1">
-        <v>1316</v>
+        <v>6515</v>
       </c>
       <c r="H9" s="1">
-        <v>1535</v>
+        <v>7818</v>
       </c>
       <c r="I9" s="1" t="str">
-        <f t="shared" ref="I9:I22" si="5">D9&amp;","&amp;E9&amp;","&amp;F9&amp;","&amp;G9&amp;","&amp;H9</f>
-        <v>658,877,1097,1316,1535</v>
-      </c>
-      <c r="J9" s="1">
-        <f t="shared" si="4"/>
-        <v>6580</v>
-      </c>
-      <c r="K9" s="1">
-        <f t="shared" si="0"/>
-        <v>8770</v>
-      </c>
-      <c r="L9" s="1">
-        <f t="shared" si="1"/>
-        <v>10970</v>
-      </c>
-      <c r="M9" s="1">
-        <f t="shared" si="2"/>
-        <v>13160</v>
-      </c>
-      <c r="N9" s="1">
-        <f t="shared" si="3"/>
-        <v>15350</v>
-      </c>
-      <c r="O9" s="1" t="str">
-        <f t="shared" ref="O9:O22" si="6">J9&amp;","&amp;K9&amp;","&amp;L9&amp;","&amp;M9&amp;","&amp;N9</f>
-        <v>6580,8770,10970,13160,15350</v>
-      </c>
-      <c r="P9" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" customHeight="1" spans="3:16">
+        <f t="shared" ref="I9:I22" si="0">D9&amp;","&amp;E9&amp;","&amp;F9&amp;","&amp;G9&amp;","&amp;H9</f>
+        <v>2606,3909,5212,6515,7818</v>
+      </c>
+      <c r="J9" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" customHeight="1" spans="3:10">
       <c r="C10" s="5">
         <v>3</v>
       </c>
       <c r="D10" s="1">
-        <v>2029</v>
+        <v>4252</v>
       </c>
       <c r="E10" s="1">
-        <v>2705</v>
+        <v>6378</v>
       </c>
       <c r="F10" s="7">
-        <v>3382</v>
+        <v>8504</v>
       </c>
       <c r="G10" s="1">
-        <v>4058</v>
+        <v>10629</v>
       </c>
       <c r="H10" s="1">
-        <v>4734</v>
+        <v>12755</v>
       </c>
       <c r="I10" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>2029,2705,3382,4058,4734</v>
-      </c>
-      <c r="J10" s="1">
-        <f t="shared" si="4"/>
-        <v>20290</v>
-      </c>
-      <c r="K10" s="1">
         <f t="shared" si="0"/>
-        <v>27050</v>
-      </c>
-      <c r="L10" s="1">
-        <f t="shared" si="1"/>
-        <v>33820</v>
-      </c>
-      <c r="M10" s="1">
-        <f t="shared" si="2"/>
-        <v>40580</v>
-      </c>
-      <c r="N10" s="1">
-        <f t="shared" si="3"/>
-        <v>47340</v>
-      </c>
-      <c r="O10" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>20290,27050,33820,40580,47340</v>
-      </c>
-      <c r="P10" s="7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" customHeight="1" spans="3:16">
+        <v>4252,6378,8504,10629,12755</v>
+      </c>
+      <c r="J10" s="7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" customHeight="1" spans="3:10">
       <c r="C11" s="5">
         <v>4</v>
       </c>
       <c r="D11" s="1">
-        <v>5176</v>
+        <v>6328</v>
       </c>
       <c r="E11" s="1">
-        <v>6901</v>
+        <v>9492</v>
       </c>
       <c r="F11" s="7">
-        <v>8627</v>
+        <v>12656</v>
       </c>
       <c r="G11" s="1">
-        <v>10352</v>
+        <v>15819</v>
       </c>
       <c r="H11" s="1">
-        <v>12077</v>
+        <v>18983</v>
       </c>
       <c r="I11" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>5176,6901,8627,10352,12077</v>
-      </c>
-      <c r="J11" s="1">
-        <f t="shared" si="4"/>
-        <v>51760</v>
-      </c>
-      <c r="K11" s="1">
         <f t="shared" si="0"/>
-        <v>69010</v>
-      </c>
-      <c r="L11" s="1">
-        <f t="shared" si="1"/>
-        <v>86270</v>
-      </c>
-      <c r="M11" s="1">
-        <f t="shared" si="2"/>
-        <v>103520</v>
-      </c>
-      <c r="N11" s="1">
-        <f t="shared" si="3"/>
-        <v>120770</v>
-      </c>
-      <c r="O11" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>51760,69010,86270,103520,120770</v>
-      </c>
-      <c r="P11" s="7">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" customHeight="1" spans="3:16">
+        <v>6328,9492,12656,15819,18983</v>
+      </c>
+      <c r="J11" s="7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" customHeight="1" spans="3:10">
       <c r="C12" s="5">
         <v>5</v>
       </c>
       <c r="D12" s="1">
-        <v>11251</v>
+        <v>9008</v>
       </c>
       <c r="E12" s="1">
-        <v>15001</v>
+        <v>13512</v>
       </c>
       <c r="F12" s="7">
-        <v>18752</v>
+        <v>18016</v>
       </c>
       <c r="G12" s="1">
-        <v>22502</v>
+        <v>22519</v>
       </c>
       <c r="H12" s="1">
-        <v>26252</v>
+        <v>27023</v>
       </c>
       <c r="I12" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>11251,15001,18752,22502,26252</v>
-      </c>
-      <c r="J12" s="1">
-        <f t="shared" si="4"/>
-        <v>112510</v>
-      </c>
-      <c r="K12" s="1">
         <f t="shared" si="0"/>
-        <v>150010</v>
-      </c>
-      <c r="L12" s="1">
-        <f t="shared" si="1"/>
-        <v>187520</v>
-      </c>
-      <c r="M12" s="1">
-        <f t="shared" si="2"/>
-        <v>225020</v>
-      </c>
-      <c r="N12" s="1">
-        <f t="shared" si="3"/>
-        <v>262520</v>
-      </c>
-      <c r="O12" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>112510,150010,187520,225020,262520</v>
-      </c>
-      <c r="P12" s="7">
+        <v>9008,13512,18016,22519,27023</v>
+      </c>
+      <c r="J12" s="7">
         <v>20</v>
       </c>
     </row>
-    <row r="13" customHeight="1" spans="3:16">
+    <row r="13" customHeight="1" spans="3:10">
       <c r="C13" s="5">
         <v>6</v>
       </c>
       <c r="D13" s="1">
-        <v>21694</v>
+        <v>12480</v>
       </c>
       <c r="E13" s="1">
-        <v>28925</v>
+        <v>18720</v>
       </c>
       <c r="F13" s="7">
-        <v>36157</v>
+        <v>24959</v>
       </c>
       <c r="G13" s="1">
-        <v>43388</v>
+        <v>31198</v>
       </c>
       <c r="H13" s="1">
-        <v>50619</v>
+        <v>37438</v>
       </c>
       <c r="I13" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>21694,28925,36157,43388,50619</v>
-      </c>
-      <c r="J13" s="1">
-        <f t="shared" si="4"/>
-        <v>216940</v>
-      </c>
-      <c r="K13" s="1">
         <f t="shared" si="0"/>
-        <v>289250</v>
-      </c>
-      <c r="L13" s="1">
-        <f t="shared" si="1"/>
-        <v>361570</v>
-      </c>
-      <c r="M13" s="1">
-        <f t="shared" si="2"/>
-        <v>433880</v>
-      </c>
-      <c r="N13" s="1">
-        <f t="shared" si="3"/>
-        <v>506190</v>
-      </c>
-      <c r="O13" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>216940,289250,361570,433880,506190</v>
-      </c>
-      <c r="P13" s="7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" customHeight="1" spans="3:16">
+        <v>12480,18720,24959,31198,37438</v>
+      </c>
+      <c r="J13" s="7">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" customHeight="1" spans="3:10">
       <c r="C14" s="5">
         <v>7</v>
       </c>
       <c r="D14" s="1">
-        <v>38233</v>
+        <v>16943</v>
       </c>
       <c r="E14" s="1">
-        <v>50977</v>
+        <v>25415</v>
       </c>
       <c r="F14" s="7">
-        <v>63722</v>
+        <v>33885</v>
       </c>
       <c r="G14" s="1">
-        <v>76466</v>
+        <v>42356</v>
       </c>
       <c r="H14" s="1">
-        <v>89210</v>
+        <v>50827</v>
       </c>
       <c r="I14" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>38233,50977,63722,76466,89210</v>
-      </c>
-      <c r="J14" s="1">
-        <f t="shared" si="4"/>
-        <v>382330</v>
-      </c>
-      <c r="K14" s="1">
         <f t="shared" si="0"/>
-        <v>509770</v>
-      </c>
-      <c r="L14" s="1">
-        <f t="shared" si="1"/>
-        <v>637220</v>
-      </c>
-      <c r="M14" s="1">
-        <f t="shared" si="2"/>
-        <v>764660</v>
-      </c>
-      <c r="N14" s="1">
-        <f t="shared" si="3"/>
-        <v>892100</v>
-      </c>
-      <c r="O14" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>382330,509770,637220,764660,892100</v>
-      </c>
-      <c r="P14" s="7">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" customHeight="1" spans="3:16">
+        <v>16943,25415,33885,42356,50827</v>
+      </c>
+      <c r="J14" s="7">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" customHeight="1" spans="3:10">
       <c r="C15" s="5">
         <v>8</v>
       </c>
       <c r="D15" s="1">
-        <v>62884</v>
+        <v>22609</v>
       </c>
       <c r="E15" s="1">
-        <v>83845</v>
+        <v>33914</v>
       </c>
       <c r="F15" s="7">
-        <v>104807</v>
+        <v>45217</v>
       </c>
       <c r="G15" s="1">
-        <v>125768</v>
+        <v>56521</v>
       </c>
       <c r="H15" s="1">
-        <v>146729</v>
+        <v>67825</v>
       </c>
       <c r="I15" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>62884,83845,104807,125768,146729</v>
-      </c>
-      <c r="J15" s="1">
-        <f t="shared" si="4"/>
-        <v>628840</v>
-      </c>
-      <c r="K15" s="1">
         <f t="shared" si="0"/>
-        <v>838450</v>
-      </c>
-      <c r="L15" s="1">
-        <f t="shared" si="1"/>
-        <v>1048070</v>
-      </c>
-      <c r="M15" s="1">
-        <f t="shared" si="2"/>
-        <v>1257680</v>
-      </c>
-      <c r="N15" s="1">
-        <f t="shared" si="3"/>
-        <v>1467290</v>
-      </c>
-      <c r="O15" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>628840,838450,1048070,1257680,1467290</v>
-      </c>
-      <c r="P15" s="7">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" customHeight="1" spans="3:16">
+        <v>22609,33914,45217,56521,67825</v>
+      </c>
+      <c r="J15" s="7">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" customHeight="1" spans="3:10">
       <c r="C16" s="5">
         <v>9</v>
       </c>
       <c r="D16" s="1">
-        <v>97951</v>
+        <v>29699</v>
       </c>
       <c r="E16" s="1">
-        <v>130601</v>
+        <v>44549</v>
       </c>
       <c r="F16" s="7">
-        <v>163252</v>
+        <v>59397</v>
       </c>
       <c r="G16" s="1">
-        <v>195902</v>
+        <v>74246</v>
       </c>
       <c r="H16" s="1">
-        <v>228552</v>
+        <v>89095</v>
       </c>
       <c r="I16" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>97951,130601,163252,195902,228552</v>
-      </c>
-      <c r="J16" s="1">
-        <f t="shared" si="4"/>
-        <v>979510</v>
-      </c>
-      <c r="K16" s="1">
         <f t="shared" si="0"/>
-        <v>1306010</v>
-      </c>
-      <c r="L16" s="1">
-        <f t="shared" si="1"/>
-        <v>1632520</v>
-      </c>
-      <c r="M16" s="1">
-        <f t="shared" si="2"/>
-        <v>1959020</v>
-      </c>
-      <c r="N16" s="1">
-        <f t="shared" si="3"/>
-        <v>2285520</v>
-      </c>
-      <c r="O16" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>979510,1306010,1632520,1959020,2285520</v>
-      </c>
-      <c r="P16" s="7">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" customHeight="1" spans="3:16">
+        <v>29699,44549,59397,74246,89095</v>
+      </c>
+      <c r="J16" s="7">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" customHeight="1" spans="3:10">
       <c r="C17" s="5">
         <v>10</v>
       </c>
       <c r="D17" s="1">
-        <v>146026</v>
+        <v>38444</v>
       </c>
       <c r="E17" s="1">
-        <v>194701</v>
+        <v>57666</v>
       </c>
       <c r="F17" s="7">
-        <v>243377</v>
+        <v>76886</v>
       </c>
       <c r="G17" s="1">
-        <v>292052</v>
+        <v>96108</v>
       </c>
       <c r="H17" s="1">
-        <v>340727</v>
+        <v>115329</v>
       </c>
       <c r="I17" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>146026,194701,243377,292052,340727</v>
-      </c>
-      <c r="J17" s="1">
-        <f t="shared" si="4"/>
-        <v>1460260</v>
-      </c>
-      <c r="K17" s="1">
         <f t="shared" si="0"/>
-        <v>1947010</v>
-      </c>
-      <c r="L17" s="1">
-        <f t="shared" si="1"/>
-        <v>2433770</v>
-      </c>
-      <c r="M17" s="1">
-        <f t="shared" si="2"/>
-        <v>2920520</v>
-      </c>
-      <c r="N17" s="1">
-        <f t="shared" si="3"/>
-        <v>3407270</v>
-      </c>
-      <c r="O17" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>1460260,1947010,2433770,2920520,3407270</v>
-      </c>
-      <c r="P17" s="7">
+        <v>38444,57666,76886,96108,115329</v>
+      </c>
+      <c r="J17" s="7">
         <v>40</v>
       </c>
     </row>
-    <row r="18" customHeight="1" spans="3:16">
+    <row r="18" customHeight="1" spans="3:10">
       <c r="C18" s="5">
         <v>11</v>
       </c>
       <c r="D18" s="1">
-        <v>209989</v>
+        <v>49083</v>
       </c>
       <c r="E18" s="1">
-        <v>279985</v>
+        <v>73624</v>
       </c>
       <c r="F18" s="7">
-        <v>349982</v>
+        <v>98163</v>
       </c>
       <c r="G18" s="1">
-        <v>419978</v>
+        <v>122704</v>
       </c>
       <c r="H18" s="1">
-        <v>489974</v>
+        <v>147245</v>
       </c>
       <c r="I18" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>209989,279985,349982,419978,489974</v>
-      </c>
-      <c r="J18" s="1">
-        <f t="shared" si="4"/>
-        <v>2099890</v>
-      </c>
-      <c r="K18" s="1">
         <f t="shared" si="0"/>
-        <v>2799850</v>
-      </c>
-      <c r="L18" s="1">
-        <f t="shared" si="1"/>
-        <v>3499820</v>
-      </c>
-      <c r="M18" s="1">
-        <f t="shared" si="2"/>
-        <v>4199780</v>
-      </c>
-      <c r="N18" s="1">
-        <f t="shared" si="3"/>
-        <v>4899740</v>
-      </c>
-      <c r="O18" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>2099890,2799850,3499820,4199780,4899740</v>
-      </c>
-      <c r="P18" s="7">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" customHeight="1" spans="3:16">
+        <v>49083,73624,98163,122704,147245</v>
+      </c>
+      <c r="J18" s="7">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" customHeight="1" spans="3:10">
       <c r="C19" s="5">
         <v>12</v>
       </c>
       <c r="D19" s="1">
-        <v>293008</v>
+        <v>61863</v>
       </c>
       <c r="E19" s="1">
-        <v>390677</v>
+        <v>92794</v>
       </c>
       <c r="F19" s="7">
-        <v>488347</v>
+        <v>123723</v>
       </c>
       <c r="G19" s="1">
-        <v>586016</v>
+        <v>154654</v>
       </c>
       <c r="H19" s="1">
-        <v>683685</v>
+        <v>185585</v>
       </c>
       <c r="I19" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>293008,390677,488347,586016,683685</v>
-      </c>
-      <c r="J19" s="1">
-        <f t="shared" si="4"/>
-        <v>2930080</v>
-      </c>
-      <c r="K19" s="1">
         <f t="shared" si="0"/>
-        <v>3906770</v>
-      </c>
-      <c r="L19" s="1">
-        <f t="shared" si="1"/>
-        <v>4883470</v>
-      </c>
-      <c r="M19" s="1">
-        <f t="shared" si="2"/>
-        <v>5860160</v>
-      </c>
-      <c r="N19" s="1">
-        <f t="shared" si="3"/>
-        <v>6836850</v>
-      </c>
-      <c r="O19" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>2930080,3906770,4883470,5860160,6836850</v>
-      </c>
-      <c r="P19" s="7">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" customHeight="1" spans="3:16">
+        <v>61863,92794,123723,154654,185585</v>
+      </c>
+      <c r="J19" s="7">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" customHeight="1" spans="3:10">
       <c r="C20" s="5">
         <v>13</v>
       </c>
       <c r="D20" s="1">
-        <v>398539</v>
+        <v>77040</v>
       </c>
       <c r="E20" s="1">
-        <v>531385</v>
+        <v>115559</v>
       </c>
       <c r="F20" s="7">
-        <v>664232</v>
+        <v>154076</v>
       </c>
       <c r="G20" s="1">
-        <v>797078</v>
+        <v>192595</v>
       </c>
       <c r="H20" s="1">
-        <v>929924</v>
+        <v>231114</v>
       </c>
       <c r="I20" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>398539,531385,664232,797078,929924</v>
-      </c>
-      <c r="J20" s="1">
-        <f t="shared" si="4"/>
-        <v>3985390</v>
-      </c>
-      <c r="K20" s="1">
         <f t="shared" si="0"/>
-        <v>5313850</v>
-      </c>
-      <c r="L20" s="1">
-        <f t="shared" si="1"/>
-        <v>6642320</v>
-      </c>
-      <c r="M20" s="1">
-        <f t="shared" si="2"/>
-        <v>7970780</v>
-      </c>
-      <c r="N20" s="1">
-        <f t="shared" si="3"/>
-        <v>9299240</v>
-      </c>
-      <c r="O20" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>3985390,5313850,6642320,7970780,9299240</v>
-      </c>
-      <c r="P20" s="7">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" customHeight="1" spans="3:16">
+        <v>77040,115559,154076,192595,231114</v>
+      </c>
+      <c r="J20" s="7">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" customHeight="1" spans="3:10">
       <c r="C21" s="5">
         <v>14</v>
       </c>
       <c r="D21" s="1">
-        <v>530326</v>
+        <v>94876</v>
       </c>
       <c r="E21" s="1">
-        <v>707101</v>
+        <v>142312</v>
       </c>
       <c r="F21" s="7">
-        <v>883877</v>
+        <v>189747</v>
       </c>
       <c r="G21" s="1">
-        <v>1060652</v>
+        <v>237183</v>
       </c>
       <c r="H21" s="1">
-        <v>1237427</v>
+        <v>284620</v>
       </c>
       <c r="I21" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>530326,707101,883877,1060652,1237427</v>
-      </c>
-      <c r="J21" s="1">
-        <f t="shared" si="4"/>
-        <v>5303260</v>
-      </c>
-      <c r="K21" s="1">
         <f t="shared" si="0"/>
-        <v>7071010</v>
-      </c>
-      <c r="L21" s="1">
-        <f t="shared" si="1"/>
-        <v>8838770</v>
-      </c>
-      <c r="M21" s="1">
-        <f t="shared" si="2"/>
-        <v>10606520</v>
-      </c>
-      <c r="N21" s="1">
-        <f t="shared" si="3"/>
-        <v>12374270</v>
-      </c>
-      <c r="O21" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>5303260,7071010,8838770,10606520,12374270</v>
-      </c>
-      <c r="P21" s="8">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" customHeight="1" spans="3:16">
+        <v>94876,142312,189747,237183,284620</v>
+      </c>
+      <c r="J21" s="8">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" customHeight="1" spans="3:10">
       <c r="C22" s="5">
         <v>15</v>
       </c>
       <c r="D22" s="1">
-        <v>692401</v>
+        <v>115640</v>
       </c>
       <c r="E22" s="1">
-        <v>923201</v>
+        <v>173457</v>
       </c>
       <c r="F22" s="8">
-        <v>1154002</v>
+        <v>231274</v>
       </c>
       <c r="G22" s="1">
-        <v>1384802</v>
+        <v>289092</v>
       </c>
       <c r="H22" s="1">
-        <v>1615602</v>
+        <v>346910</v>
       </c>
       <c r="I22" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>692401,923201,1154002,1384802,1615602</v>
+        <f t="shared" si="0"/>
+        <v>115640,173457,231274,289092,346910</v>
       </c>
       <c r="J22" s="1">
-        <f t="shared" si="4"/>
-        <v>6924010</v>
-      </c>
-      <c r="K22" s="1">
-        <f t="shared" si="0"/>
-        <v>9232010</v>
-      </c>
-      <c r="L22" s="1">
-        <f t="shared" si="1"/>
-        <v>11540020</v>
-      </c>
-      <c r="M22" s="1">
-        <f t="shared" si="2"/>
-        <v>13848020</v>
-      </c>
-      <c r="N22" s="1">
-        <f t="shared" si="3"/>
-        <v>16156020</v>
-      </c>
-      <c r="O22" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>6924010,9232010,11540020,13848020,16156020</v>
-      </c>
-      <c r="P22" s="1">
         <v>60</v>
       </c>
     </row>

</xml_diff>